<commit_message>
Update Excel file for Systems Engineering work
</commit_message>
<xml_diff>
--- a/Systems Engineering/work1/2025.12.18 栁原魁人.xlsx
+++ b/Systems Engineering/work1/2025.12.18 栁原魁人.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaito\TeX-Folder\Systems Engineering\work1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B141234C-DE56-4784-B050-319D18826E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05FD4385-35A7-4386-9926-59F5ADE03024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14310" yWindow="0" windowWidth="14580" windowHeight="17370" xr2:uid="{2D9D279B-0571-4FC0-86AD-69BD68A62247}"/>
+    <workbookView xWindow="4550" yWindow="4610" windowWidth="21600" windowHeight="12670" xr2:uid="{2D9D279B-0571-4FC0-86AD-69BD68A62247}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,9 +92,6 @@
     <t>【課題①】標準偏差</t>
   </si>
   <si>
-    <t>【課題②】工程能力指数(Cpk)</t>
-  </si>
-  <si>
     <t>【課題⑤】推測される課題およびその根拠</t>
   </si>
   <si>
@@ -181,6 +178,10 @@
   </si>
   <si>
     <t>データ10(μm)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>【課題②】工程能力指数(Cp)</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -284,37 +285,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="ja-JP"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -918,6 +889,47 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ja-JP"/>
+              <a:t>【</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ja-JP" altLang="en-US"/>
+              <a:t>課題②</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ja-JP"/>
+              <a:t>】</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ja-JP" altLang="en-US"/>
+              <a:t>工程能力指数</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ja-JP"/>
+              <a:t>(Cp)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -962,7 +974,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>【課題②】工程能力指数(Cpk)</c:v>
+                  <c:v>【課題②】工程能力指数(Cp)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2769,8 +2781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09A574E5-839E-4BA8-9F68-7A27432ABACC}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -2780,7 +2792,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -2850,37 +2862,37 @@
     </row>
     <row r="3" spans="1:11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
         <v>33</v>
       </c>
-      <c r="B3" t="s">
-        <v>34</v>
-      </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
@@ -2920,7 +2932,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="1">
         <v>0.08</v>
@@ -2955,7 +2967,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1">
         <v>0.05</v>
@@ -2990,7 +3002,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" s="1">
         <v>0.12</v>
@@ -3025,7 +3037,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B8" s="1">
         <v>7.0000000000000007E-2</v>
@@ -3060,7 +3072,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="1">
         <v>0.15</v>
@@ -3095,7 +3107,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="1">
         <v>0.03</v>
@@ -3130,7 +3142,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="1">
         <v>0.11</v>
@@ -3165,7 +3177,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1">
         <v>0.02</v>
@@ -3200,7 +3212,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="1">
         <v>0.09</v>
@@ -3235,7 +3247,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" s="1">
         <v>0.05</v>
@@ -3450,7 +3462,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="B19" s="1">
         <f>(B2-B17)/(3*B18)</f>
@@ -3495,67 +3507,67 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>